<commit_message>
reorganize and updated analyses
</commit_message>
<xml_diff>
--- a/Data/PreliminaryProteomeCharacterization.xlsx
+++ b/Data/PreliminaryProteomeCharacterization.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Shelly/Documents/GitHub/OysterSeedProject/analysis/UniprotAnnotations_NetworkAnalysis/General_proteome_characterization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1B081E-1FFF-0248-89FB-29EF3EE07A85}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C7453A-C5F6-8A47-B086-7BB343147686}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3140" yWindow="1160" windowWidth="21060" windowHeight="11020" xr2:uid="{E4D4141F-9E7A-AF49-93CF-6C29E7FAD514}"/>
+    <workbookView xWindow="1560" yWindow="7720" windowWidth="21060" windowHeight="11020" xr2:uid="{E4D4141F-9E7A-AF49-93CF-6C29E7FAD514}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">Exposure Day </t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>29C</t>
+  </si>
+  <si>
+    <t>Days post fertilization</t>
   </si>
 </sst>
 </file>
@@ -164,22 +167,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -248,22 +251,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -332,22 +335,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -426,13 +429,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>days exposed</a:t>
+                  <a:t>days post-fertilization</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> to increased temperature</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1606,10 +1604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26FE76AD-3FF5-BB4E-94DC-91D3CCBB3FEE}">
-  <dimension ref="B1:E7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1617,9 +1615,12 @@
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -1631,9 +1632,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>3</v>
+      </c>
       <c r="B2">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C2">
         <v>904</v>
@@ -1645,9 +1649,12 @@
         <v>738</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>5</v>
+      </c>
       <c r="B3">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="C3">
         <v>913</v>
@@ -1659,9 +1666,12 @@
         <v>629</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>7</v>
+      </c>
       <c r="B4">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="C4">
         <v>906</v>
@@ -1673,9 +1683,12 @@
         <v>573</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>9</v>
+      </c>
       <c r="B5">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="C5">
         <v>1005</v>
@@ -1687,9 +1700,12 @@
         <v>655</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>11</v>
+      </c>
       <c r="B6">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="C6">
         <v>807</v>
@@ -1701,9 +1717,12 @@
         <v>705</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>13</v>
+      </c>
       <c r="B7">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="C7">
         <v>561</v>

</xml_diff>